<commit_message>
RRO-1010 - Refine light armor stats
</commit_message>
<xml_diff>
--- a/tools/Spreadsheet/Armor 5.0.0 vs 5.1.0.xlsx
+++ b/tools/Spreadsheet/Armor 5.0.0 vs 5.1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem-special-edition\tools\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF26F1E-23C1-45CD-9753-E635663C31C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D5AC8C-C128-4CC6-B492-1E339FF9F84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B9ECBDAD-DB74-42BC-9A1E-CA4CBE361830}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B9ECBDAD-DB74-42BC-9A1E-CA4CBE361830}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="61">
   <si>
     <t>Aetherium</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Buff</t>
+  </si>
+  <si>
+    <t>Executioner</t>
+  </si>
+  <si>
+    <t>Scale</t>
   </si>
 </sst>
 </file>
@@ -566,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB908B8-366A-4A32-A57D-1E546DC4B63F}">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,10 +2340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5631F2-CBFB-4A6A-8470-C61F6D6DDEC1}">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,7 +2421,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M29" si="0">IF(B2&lt;&gt;"", H2 - B2 - K2, "")</f>
+        <f t="shared" ref="M2:M30" si="0">IF(B2&lt;&gt;"", H2 - B2 - K2, "")</f>
         <v>0</v>
       </c>
       <c r="N2">
@@ -2444,15 +2450,15 @@
         <v>10</v>
       </c>
       <c r="V2" t="str">
-        <f t="shared" ref="V2:V29" si="1">IF(A2=S2,"",FALSE)</f>
+        <f t="shared" ref="V2:V30" si="1">IF(A2=S2,"",FALSE)</f>
         <v/>
       </c>
       <c r="W2" t="str">
-        <f t="shared" ref="W2:W29" si="2">IF(H2=T2,"",FALSE)</f>
+        <f t="shared" ref="W2:W30" si="2">IF(H2=T2,"",FALSE)</f>
         <v/>
       </c>
       <c r="X2" t="str">
-        <f t="shared" ref="X2:X29" si="3">IF(I2=U2,"",FALSE)</f>
+        <f t="shared" ref="X2:X30" si="3">IF(I2=U2,"",FALSE)</f>
         <v/>
       </c>
     </row>
@@ -2489,19 +2495,19 @@
         <v>-10</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N29" si="4">IF(C3&lt;&gt;"", I3 - C3, "")</f>
+        <f t="shared" ref="N3:N30" si="4">IF(C3&lt;&gt;"", I3 - C3, "")</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O29" si="5">IF(D3&lt;&gt;"", H3-(B3+D3*60), "")</f>
+        <f t="shared" ref="O3:O30" si="5">IF(D3&lt;&gt;"", H3-(B3+D3*60), "")</f>
         <v>-70</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P29" si="6">IF(E3&lt;&gt;"", H3-(B3+E3*60), "")</f>
+        <f t="shared" ref="P3:P30" si="6">IF(E3&lt;&gt;"", H3-(B3+E3*60), "")</f>
         <v>-10</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q29" si="7">IF(F3&lt;&gt;"", (H3+J3*50)-(B3+F3*60),"")</f>
+        <f t="shared" ref="Q3:Q30" si="7">IF(F3&lt;&gt;"", (H3+J3*50)-(B3+F3*60),"")</f>
         <v>130</v>
       </c>
       <c r="S3" t="s">
@@ -2549,7 +2555,7 @@
         <v>400</v>
       </c>
       <c r="I4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -2560,7 +2566,7 @@
       </c>
       <c r="N4">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O4">
         <f t="shared" si="5"/>
@@ -2581,7 +2587,7 @@
         <v>400</v>
       </c>
       <c r="U4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="V4" t="str">
         <f t="shared" si="1"/>
@@ -2624,12 +2630,9 @@
       <c r="J5">
         <v>2</v>
       </c>
-      <c r="K5">
-        <v>100</v>
-      </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
@@ -2814,115 +2817,59 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>250</v>
-      </c>
-      <c r="I8">
-        <v>15</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="Q8" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <v>59</v>
       </c>
       <c r="S8" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="T8">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U8">
-        <v>15</v>
-      </c>
-      <c r="V8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9">
-        <v>250</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H9">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="I9">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>2</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="S9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="T9">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="U9">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="1"/>
@@ -2939,7 +2886,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>250</v>
@@ -2986,7 +2933,7 @@
         <v>-10</v>
       </c>
       <c r="S10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T10">
         <v>250</v>
@@ -3009,42 +2956,39 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
-        <v>480</v>
+        <v>250</v>
       </c>
       <c r="C11">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="I11">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <f t="shared" si="5"/>
@@ -3052,20 +2996,20 @@
       </c>
       <c r="P11">
         <f t="shared" si="6"/>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="Q11">
         <f t="shared" si="7"/>
-        <v>90</v>
+        <v>-10</v>
       </c>
       <c r="S11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T11">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="U11">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="1"/>
@@ -3082,60 +3026,63 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B12">
-        <v>300</v>
+        <v>480</v>
       </c>
       <c r="C12">
         <v>15</v>
       </c>
       <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
       <c r="H12">
-        <v>300</v>
+        <v>550</v>
       </c>
       <c r="I12">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O12">
         <f t="shared" si="5"/>
-        <v>-180</v>
+        <v>-50</v>
       </c>
       <c r="P12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="Q12">
         <f t="shared" si="7"/>
-        <v>-70</v>
+        <v>40</v>
       </c>
       <c r="S12" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="T12">
-        <v>300</v>
+        <v>550</v>
       </c>
       <c r="U12">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="1"/>
@@ -3152,28 +3099,28 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C13">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="I13">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -3188,7 +3135,7 @@
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-180</v>
       </c>
       <c r="P13">
         <f t="shared" si="6"/>
@@ -3196,16 +3143,16 @@
       </c>
       <c r="Q13">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>-70</v>
       </c>
       <c r="S13" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="T13">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="U13">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="1"/>
@@ -3222,22 +3169,22 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B14">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>300</v>
@@ -3250,26 +3197,26 @@
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O14">
         <f t="shared" si="5"/>
-        <v>-60</v>
+        <v>50</v>
       </c>
       <c r="P14">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q14">
         <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>100</v>
       </c>
       <c r="S14" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="T14">
         <v>300</v>
@@ -3292,7 +3239,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>300</v>
@@ -3339,7 +3286,7 @@
         <v>-10</v>
       </c>
       <c r="S15" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="T15">
         <v>300</v>
@@ -3362,7 +3309,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>300</v>
@@ -3409,7 +3356,7 @@
         <v>-10</v>
       </c>
       <c r="S16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T16">
         <v>300</v>
@@ -3432,45 +3379,60 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>300</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="I17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="Q17" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="5"/>
+        <v>-60</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="7"/>
+        <v>-10</v>
       </c>
       <c r="S17" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="T17">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="U17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="1"/>
@@ -3487,60 +3449,45 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18">
-        <v>360</v>
-      </c>
-      <c r="C18">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+        <v>55</v>
+      </c>
+      <c r="H18">
+        <v>500</v>
+      </c>
+      <c r="I18">
+        <v>30</v>
+      </c>
+      <c r="J18">
         <v>2</v>
       </c>
-      <c r="H18">
-        <v>350</v>
-      </c>
-      <c r="I18">
-        <v>12</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="5"/>
-        <v>-70</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="6"/>
-        <v>-10</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="7"/>
-        <v>70</v>
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="S18" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="T18">
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="U18">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="1"/>
@@ -3557,7 +3504,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>360</v>
@@ -3569,26 +3516,23 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
       <c r="H19">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="I19">
         <v>12</v>
       </c>
       <c r="J19">
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>-10</v>
       </c>
       <c r="N19">
         <f t="shared" si="4"/>
@@ -3596,21 +3540,21 @@
       </c>
       <c r="O19">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>-70</v>
       </c>
       <c r="P19">
         <f t="shared" si="6"/>
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="Q19">
         <f t="shared" si="7"/>
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="S19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T19">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="U19">
         <v>12</v>
@@ -3630,45 +3574,63 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>360</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
       </c>
       <c r="H20">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I20">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="J20">
         <v>2</v>
       </c>
-      <c r="M20" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="Q20" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="6"/>
+        <v>-40</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="7"/>
+        <v>120</v>
       </c>
       <c r="S20" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="T20">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="U20">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="1"/>
@@ -3685,63 +3647,45 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21">
-        <v>360</v>
-      </c>
-      <c r="C21">
-        <v>15</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="H21">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J21">
         <v>2</v>
       </c>
-      <c r="K21">
-        <v>100</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="5"/>
-        <v>140</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="6"/>
-        <v>-40</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="7"/>
-        <v>180</v>
+      <c r="M21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="S21" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="T21">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="U21">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="1"/>
@@ -3758,64 +3702,67 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="H22">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="I22">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
       </c>
       <c r="M22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O22">
         <f t="shared" si="5"/>
-        <v>-60</v>
+        <v>140</v>
       </c>
       <c r="P22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="Q22">
         <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>180</v>
       </c>
       <c r="S22" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="T22">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="U22">
-        <v>10</v>
-      </c>
-      <c r="V22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>20</v>
+      </c>
+      <c r="V22" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="W22" t="str">
         <f t="shared" si="2"/>
@@ -3828,7 +3775,22 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>300</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
       </c>
       <c r="H23">
         <v>300</v>
@@ -3839,28 +3801,28 @@
       <c r="J23">
         <v>1</v>
       </c>
-      <c r="M23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N23" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P23" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="Q23" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="5"/>
+        <v>-60</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="7"/>
+        <v>-10</v>
       </c>
       <c r="S23" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="T23">
         <v>300</v>
@@ -3883,60 +3845,45 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24">
-        <v>480</v>
-      </c>
-      <c r="C24">
-        <v>15</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="H24">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="I24">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J24">
-        <v>3</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="6"/>
-        <v>-40</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>1</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="S24" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="T24">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="U24">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="1"/>
@@ -3953,48 +3900,60 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>480</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
       </c>
       <c r="H25">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="I25">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="J25">
         <v>3</v>
       </c>
-      <c r="K25">
-        <v>100</v>
-      </c>
-      <c r="M25" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N25" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P25" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="Q25" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="6"/>
+        <v>-40</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="7"/>
+        <v>-10</v>
       </c>
       <c r="S25" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="T25">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="U25">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="1"/>
@@ -4011,60 +3970,48 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26">
-        <v>300</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="H26">
-        <v>300</v>
+        <v>550</v>
       </c>
       <c r="I26">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="5"/>
-        <v>-60</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>3</v>
+      </c>
+      <c r="K26">
+        <v>100</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="S26" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="T26">
-        <v>300</v>
+        <v>550</v>
       </c>
       <c r="U26">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="V26" t="str">
         <f t="shared" si="1"/>
@@ -4081,13 +4028,13 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="C27">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -4099,42 +4046,42 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="I27">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="5"/>
+        <v>-60</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="7"/>
         <v>-10</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="5"/>
-        <v>-70</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="6"/>
-        <v>-10</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="7"/>
-        <v>130</v>
-      </c>
       <c r="S27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T27">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="U27">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="1"/>
@@ -4151,7 +4098,22 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="B28">
+        <v>360</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
       </c>
       <c r="H28">
         <v>350</v>
@@ -4162,28 +4124,28 @@
       <c r="J28">
         <v>4</v>
       </c>
-      <c r="M28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N28" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P28" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="Q28" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="5"/>
+        <v>-70</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="6"/>
+        <v>-10</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="7"/>
+        <v>130</v>
       </c>
       <c r="S28" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="T28">
         <v>350</v>
@@ -4206,70 +4168,125 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29">
+        <v>350</v>
+      </c>
+      <c r="I29">
+        <v>12</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="S29" t="s">
+        <v>20</v>
+      </c>
+      <c r="T29">
+        <v>350</v>
+      </c>
+      <c r="U29">
+        <v>12</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="X29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>45</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>300</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>10</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="H29">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="H30">
         <v>300</v>
       </c>
-      <c r="I29">
+      <c r="I30">
         <v>10</v>
       </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O29">
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
         <f t="shared" si="5"/>
         <v>-60</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q29">
+      <c r="P30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
         <f t="shared" si="7"/>
         <v>-10</v>
       </c>
-      <c r="S29" t="s">
+      <c r="S30" t="s">
         <v>45</v>
       </c>
-      <c r="T29">
+      <c r="T30">
         <v>300</v>
       </c>
-      <c r="U29">
+      <c r="U30">
         <v>10</v>
       </c>
-      <c r="V29" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W29" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="X29" t="str">
+      <c r="V30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="X30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>

</xml_diff>